<commit_message>
Added patient landing page and doctor list page..
</commit_message>
<xml_diff>
--- a/Sharable/DoctorsData.xlsx
+++ b/Sharable/DoctorsData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Doctors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,40 +19,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>phone 1</t>
-  </si>
-  <si>
-    <t>phone 2</t>
-  </si>
-  <si>
-    <t>Specialization</t>
-  </si>
-  <si>
-    <t>Area / Nearby Stattion</t>
-  </si>
-  <si>
     <t>Reviews</t>
   </si>
   <si>
-    <t>timmings</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Area / Nearby Station</t>
+  </si>
+  <si>
+    <t>Phone1</t>
+  </si>
+  <si>
+    <t>Phone2</t>
+  </si>
+  <si>
+    <t>Specialisation</t>
+  </si>
+  <si>
+    <t>Timings</t>
+  </si>
+  <si>
+    <t>Days of Week</t>
+  </si>
+  <si>
+    <t>Keywords for search</t>
+  </si>
+  <si>
+    <t>Dr. SUHAS C BENDRE</t>
+  </si>
+  <si>
+    <t>Vikhroli</t>
+  </si>
+  <si>
+    <t>Cardio Thorasic And Vascular</t>
+  </si>
+  <si>
+    <t>2pm to 4pm</t>
+  </si>
+  <si>
+    <t>MTWTFSS</t>
+  </si>
+  <si>
+    <t>cancer, heart,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. AMIT BHARAT SANGHVI </t>
+  </si>
+  <si>
+    <t>Powai</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9am to 12pm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. DILIP V MAYDEO </t>
+  </si>
+  <si>
+    <t>Mulund</t>
+  </si>
+  <si>
+    <t>Chest Physician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9am to 11am </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. BHARTI V KHANDEKAR </t>
+  </si>
+  <si>
+    <t>Lower Parel</t>
+  </si>
+  <si>
+    <t>Cleft Clinic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12pm to 2pm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. NAZREEN SHAIKH </t>
+  </si>
+  <si>
+    <t>Andheri</t>
+  </si>
+  <si>
+    <t>Clinical Psychology</t>
+  </si>
+  <si>
+    <t>2pm to 5pm</t>
+  </si>
+  <si>
+    <t>Dr. JEEVAN S SHETTY</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>1pm to 2pm &amp; 5pm to 7pm</t>
+  </si>
+  <si>
+    <t>Dr. HARIHARAN KRISHANAN</t>
+  </si>
+  <si>
+    <t>Borivali</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11am to 12pm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. ABHIJIT ASHOK JADHAV </t>
+  </si>
+  <si>
+    <t>Ghatkopar</t>
+  </si>
+  <si>
+    <t>Diabetology</t>
+  </si>
+  <si>
+    <t>3pm to 5pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. JITEN CHOWDHRY </t>
+  </si>
+  <si>
+    <t>Dadar</t>
+  </si>
+  <si>
+    <t>General Surgery</t>
+  </si>
+  <si>
+    <t>9am to 2pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr. ADITI SINGHI </t>
+  </si>
+  <si>
+    <t>Gynaecology</t>
+  </si>
+  <si>
+    <t>6pm to 7pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,6 +200,25 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -113,8 +258,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -462,44 +622,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I2"/>
+  <dimension ref="A2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="11" max="11" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E3" s="4">
+        <v>91</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="42">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E4" s="4">
+        <v>92</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E5" s="4">
+        <v>93</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="42">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E6" s="4">
+        <v>94</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="42">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E7" s="4">
+        <v>95</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="42">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E8" s="4">
+        <v>96</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="42">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E9" s="4">
+        <v>97</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="42">
+      <c r="A10" s="4">
         <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E10" s="4">
+        <v>98</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E11" s="4">
+        <v>99</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4">
+        <f>91</f>
+        <v>91</v>
+      </c>
+      <c r="E12" s="4">
+        <v>100</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added doctors search list page and doctors details page
Added doctors search list page and doctors details page
Improved the navigation structure and Activity to Fragments
communication.
</commit_message>
<xml_diff>
--- a/Sharable/DoctorsData.xlsx
+++ b/Sharable/DoctorsData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -625,7 +625,7 @@
   <dimension ref="A2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -726,9 +726,7 @@
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="H4" s="4"/>
       <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
@@ -759,9 +757,7 @@
       <c r="G5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="H5" s="4"/>
       <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
@@ -792,9 +788,7 @@
       <c r="G6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="H6" s="4"/>
       <c r="I6" s="5" t="s">
         <v>28</v>
       </c>
@@ -825,9 +819,7 @@
       <c r="G7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="H7" s="4"/>
       <c r="I7" s="5" t="s">
         <v>32</v>
       </c>
@@ -858,9 +850,7 @@
       <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="H8" s="4"/>
       <c r="I8" s="5" t="s">
         <v>35</v>
       </c>
@@ -891,9 +881,7 @@
       <c r="G9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="H9" s="4"/>
       <c r="I9" s="5" t="s">
         <v>39</v>
       </c>
@@ -924,9 +912,7 @@
       <c r="G10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
         <v>43</v>
       </c>
@@ -957,9 +943,7 @@
       <c r="G11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="H11" s="4"/>
       <c r="I11" s="5" t="s">
         <v>47</v>
       </c>
@@ -990,9 +974,7 @@
       <c r="G12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
         <v>50</v>
       </c>

</xml_diff>